<commit_message>
Manual testing notes on june 14th
</commit_message>
<xml_diff>
--- a/Test Scenario Template.xlsx
+++ b/Test Scenario Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\010LiveTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35F1C1D-047F-4D7F-B61E-987D4738075A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C5475-9C7B-4CA9-8C33-9ECAB126B75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{53FC4BEA-8F91-4E79-BF52-DCF5852BF4C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{53FC4BEA-8F91-4E79-BF52-DCF5852BF4C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios for Adactin" sheetId="1" r:id="rId1"/>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F7028C-85A9-4F85-B95C-6BAD167F50C0}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -708,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E262C7-F4D8-4A1A-BF76-19C0A4F941AD}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>